<commit_message>
Added comment for test cases added for Institute and department
SVN-Revision: 25430
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/Inst_Dept_Site_CRG_SAType_DP.xlsx
+++ b/TestCases/ToBeAutomated/Inst_Dept_Site_CRG_SAType_DP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="178">
   <si>
     <t>Test Edit Collection Protocol Title Based(beforeReg_CP_fields)</t>
   </si>
@@ -306,9 +306,6 @@
     <t>As admin</t>
   </si>
   <si>
-    <t>Mandatory_field_missing</t>
-  </si>
-  <si>
     <t>Add_institute_as_superadmin</t>
   </si>
   <si>
@@ -538,6 +535,21 @@
   </si>
   <si>
     <t>EditSAType_dimension</t>
+  </si>
+  <si>
+    <t>ID missing</t>
+  </si>
+  <si>
+    <t>Already existing name</t>
+  </si>
+  <si>
+    <t>Name missing</t>
+  </si>
+  <si>
+    <t>Already existing</t>
+  </si>
+  <si>
+    <t>Name Missing</t>
   </si>
 </sst>
 </file>
@@ -887,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D103"/>
+  <dimension ref="A2:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -904,13 +916,13 @@
   <sheetData>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="30">
       <c r="B2" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -918,7 +930,10 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -926,7 +941,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -935,6 +953,12 @@
       </c>
       <c r="B5" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -942,55 +966,94 @@
       <c r="B6" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>175</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>176</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>173</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>174</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -998,251 +1061,288 @@
       <c r="B14" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="4">
+        <v>40616</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D19" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D20" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D25" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D26" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D27" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D28" s="4">
+        <v>40616</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D30" s="4">
-        <v>40595</v>
+        <v>40616</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3"/>
+      <c r="A31" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D33" s="4">
         <v>40595</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D34" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D35" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D36" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="4">
         <v>40595</v>
@@ -1251,10 +1351,10 @@
     <row r="39" spans="1:4">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="4">
         <v>40595</v>
@@ -1263,49 +1363,55 @@
     <row r="40" spans="1:4">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D41" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D42" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D43" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3"/>
       <c r="B44" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D44" s="4">
         <v>40595</v>
@@ -1314,267 +1420,254 @@
     <row r="45" spans="1:4">
       <c r="A45" s="3"/>
       <c r="B45" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D45" s="4">
         <v>40595</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="3"/>
+      <c r="A46" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="B46" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3"/>
       <c r="B47" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="4">
-        <v>40595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3"/>
       <c r="B49" s="2" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D49" s="4">
         <v>40595</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="A50" s="3"/>
       <c r="B50" s="2" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D50" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3"/>
       <c r="B51" s="2" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D51" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3"/>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D52" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3"/>
       <c r="B53" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3"/>
       <c r="B54" s="2" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3"/>
       <c r="B55" s="2" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3"/>
       <c r="B56" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D56" s="4">
-        <v>40596</v>
+        <v>40595</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3"/>
       <c r="B57" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D57" s="4">
-        <v>40596</v>
+        <v>40595</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="3"/>
       <c r="B58" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" s="4">
-        <v>40596</v>
+        <v>40595</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3"/>
       <c r="B59" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D59" s="4">
-        <v>40596</v>
+        <v>40595</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="3"/>
       <c r="B60" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D60" s="4">
+        <v>40595</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="3"/>
       <c r="B61" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D61" s="4">
-        <v>40596</v>
+        <v>40595</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="3"/>
+      <c r="A62" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B62" s="2" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="3"/>
       <c r="B63" s="2" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D63" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="3"/>
       <c r="B64" s="2" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3"/>
       <c r="B65" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D65" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3"/>
       <c r="B66" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D66" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3"/>
       <c r="B67" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D67" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="3"/>
       <c r="B68" s="2" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" s="4">
         <v>40596</v>
@@ -1583,10 +1676,10 @@
     <row r="69" spans="1:4">
       <c r="A69" s="3"/>
       <c r="B69" s="2" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D69" s="4">
         <v>40596</v>
@@ -1595,10 +1688,10 @@
     <row r="70" spans="1:4">
       <c r="A70" s="3"/>
       <c r="B70" s="2" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D70" s="4">
         <v>40596</v>
@@ -1607,10 +1700,10 @@
     <row r="71" spans="1:4">
       <c r="A71" s="3"/>
       <c r="B71" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D71" s="4">
         <v>40596</v>
@@ -1619,19 +1712,19 @@
     <row r="72" spans="1:4">
       <c r="A72" s="3"/>
       <c r="B72" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3"/>
       <c r="B73" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D73" s="4">
         <v>40596</v>
@@ -1640,10 +1733,10 @@
     <row r="74" spans="1:4">
       <c r="A74" s="3"/>
       <c r="B74" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D74" s="4">
         <v>40596</v>
@@ -1652,10 +1745,10 @@
     <row r="75" spans="1:4">
       <c r="A75" s="3"/>
       <c r="B75" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D75" s="4">
         <v>40596</v>
@@ -1664,60 +1757,70 @@
     <row r="76" spans="1:4">
       <c r="A76" s="3"/>
       <c r="B76" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D76" s="4">
         <v>40596</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="A77" s="3"/>
       <c r="B77" s="2" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D77" s="4">
+        <v>40596</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3"/>
       <c r="B78" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D78" s="4">
+        <v>40596</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="3"/>
       <c r="B79" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D79" s="4">
+        <v>40596</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3"/>
       <c r="B80" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="D80" s="4">
+        <v>40596</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3"/>
       <c r="B81" s="2" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D81" s="4">
         <v>40596</v>
@@ -1726,10 +1829,10 @@
     <row r="82" spans="1:4">
       <c r="A82" s="3"/>
       <c r="B82" s="2" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D82" s="4">
         <v>40596</v>
@@ -1738,10 +1841,10 @@
     <row r="83" spans="1:4">
       <c r="A83" s="3"/>
       <c r="B83" s="2" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D83" s="4">
         <v>40596</v>
@@ -1750,22 +1853,19 @@
     <row r="84" spans="1:4">
       <c r="A84" s="3"/>
       <c r="B84" s="2" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D84" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3"/>
       <c r="B85" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D85" s="4">
         <v>40596</v>
@@ -1774,10 +1874,10 @@
     <row r="86" spans="1:4">
       <c r="A86" s="3"/>
       <c r="B86" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D86" s="4">
         <v>40596</v>
@@ -1786,10 +1886,10 @@
     <row r="87" spans="1:4">
       <c r="A87" s="3"/>
       <c r="B87" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D87" s="4">
         <v>40596</v>
@@ -1798,70 +1898,60 @@
     <row r="88" spans="1:4">
       <c r="A88" s="3"/>
       <c r="B88" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D88" s="4">
         <v>40596</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="3"/>
+      <c r="A89" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="B89" s="2" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3"/>
       <c r="B90" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D90" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3"/>
       <c r="B91" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D91" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="3"/>
       <c r="B92" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D92" s="4">
-        <v>40596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="3"/>
       <c r="B93" s="2" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D93" s="4">
         <v>40596</v>
@@ -1870,10 +1960,10 @@
     <row r="94" spans="1:4">
       <c r="A94" s="3"/>
       <c r="B94" s="2" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D94" s="4">
         <v>40596</v>
@@ -1882,10 +1972,10 @@
     <row r="95" spans="1:4">
       <c r="A95" s="3"/>
       <c r="B95" s="2" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D95" s="4">
         <v>40596</v>
@@ -1894,53 +1984,197 @@
     <row r="96" spans="1:4">
       <c r="A96" s="3"/>
       <c r="B96" s="2" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D96" s="4">
         <v>40596</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="3" t="s">
-        <v>115</v>
-      </c>
+    <row r="97" spans="1:4">
+      <c r="A97" s="3"/>
       <c r="B97" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="3" t="s">
-        <v>112</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="3"/>
       <c r="B98" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>162</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="3"/>
       <c r="B99" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="3"/>
+      <c r="B100" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3"/>
+      <c r="B101" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="3"/>
+      <c r="B102" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="3"/>
+      <c r="B103" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D103" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="3"/>
+      <c r="B104" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D104" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="3"/>
+      <c r="B105" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="3"/>
+      <c r="B106" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="3"/>
+      <c r="B107" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D107" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="3"/>
+      <c r="B108" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D108" s="4">
+        <v>40596</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="3"/>
+      <c r="B111" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="B100" s="2" t="s">
+    <row r="112" spans="1:4">
+      <c r="B112" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="B101" s="2" t="s">
+    <row r="113" spans="1:2">
+      <c r="B113" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B103" s="2" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" s="3" t="s">
         <v>113</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case updated for Institute and department
SVN-Revision: 25431
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/Inst_Dept_Site_CRG_SAType_DP.xlsx
+++ b/TestCases/ToBeAutomated/Inst_Dept_Site_CRG_SAType_DP.xlsx
@@ -902,7 +902,7 @@
   <dimension ref="A2:D115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,9 +1005,7 @@
       <c r="C9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="4">
-        <v>40616</v>
-      </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
@@ -1172,9 +1170,7 @@
       <c r="C23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="4">
-        <v>40616</v>
-      </c>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3"/>

</xml_diff>